<commit_message>
Revised 2019 charts. New 2020 charts.
</commit_message>
<xml_diff>
--- a/papers_duedates.xlsx
+++ b/papers_duedates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\The University of the West Indies\DataGroup - DG_Resources\DATAGROUP_outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\OneDrive - The University of the West Indies\repo_ianhambleton\repo_papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1404,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1420,7 +1420,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>43496</v>
+        <v>43466</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3">
-        <v>43503</v>
+        <v>43480</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1480,7 +1480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="3">
-        <v>43512</v>
+        <v>43496</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -1500,7 +1500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>43519</v>
+        <v>43506</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -1519,8 +1519,11 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <v>21915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>43524</v>
+        <v>43521</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1539,8 +1542,12 @@
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <f>K5+31</f>
+        <v>21946</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1559,8 +1566,12 @@
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <f>K6+28</f>
+        <v>21974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1579,8 +1590,12 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <f t="shared" ref="K7:K16" si="0">K7+31</f>
+        <v>22005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1596,8 +1611,12 @@
       <c r="F9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <f>K8+30</f>
+        <v>22035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1613,8 +1632,12 @@
       <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>22066</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1630,8 +1653,12 @@
       <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <f>K10+30</f>
+        <v>22096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1650,8 +1677,12 @@
       <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>22127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1667,8 +1698,12 @@
       <c r="F13" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>22158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1684,8 +1719,12 @@
       <c r="F14" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <f>K13+30</f>
+        <v>22188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -1701,8 +1740,12 @@
       <c r="F15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <f t="shared" si="0"/>
+        <v>22219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1717,6 +1760,10 @@
       </c>
       <c r="F16" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>22250</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2261,11 +2308,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocType xmlns="8c4c3fb4-1483-4ae0-9923-479b3a23e2d8">Not Classified</DocType>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2464,27 +2512,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocType xmlns="8c4c3fb4-1483-4ae0-9923-479b3a23e2d8">Not Classified</DocType>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECDEECEB-ADBD-4F66-A19C-F58D039BF01B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7754218-24ED-4DEF-A442-30AB630462AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9bac7cda-8c2f-43dc-b4ab-c79f0d5d96ea"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8c4c3fb4-1483-4ae0-9923-479b3a23e2d8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2509,9 +2547,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7754218-24ED-4DEF-A442-30AB630462AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECDEECEB-ADBD-4F66-A19C-F58D039BF01B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9bac7cda-8c2f-43dc-b4ab-c79f0d5d96ea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8c4c3fb4-1483-4ae0-9923-479b3a23e2d8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>